<commit_message>
"Implemented functionality of selecting test scenario, to execute or not, based upon the value of isEnabled field in the Excel sheet."
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/CreateUserDataTestScenario.xlsx
+++ b/src/test/resources/testdata/CreateUserDataTestScenario.xlsx
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="43">
+  <si>
+    <t xml:space="preserve">isEnabled</t>
+  </si>
   <si>
     <t xml:space="preserve">TestScenario</t>
   </si>
@@ -59,6 +62,9 @@
   </si>
   <si>
     <t xml:space="preserve">Create User With Existing User ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERROR</t>
   </si>
   <si>
     <t xml:space="preserve">RandomId_6</t>
@@ -149,15 +155,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -179,7 +185,6 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -224,12 +229,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -254,19 +263,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="23.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.92"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -282,7 +291,7 @@
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -291,7 +300,7 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="0" t="s">
@@ -303,178 +312,205 @@
       <c r="K1" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>11</v>
+      <c r="A2" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="0" t="n">
         <v>400</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="G2" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="I2" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="0" t="n">
+      <c r="J2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="0" t="n">
         <v>9876543210</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>19</v>
+      <c r="A3" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="0" t="n">
         <v>400</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>21</v>
+      <c r="E3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>22</v>
+      <c r="A4" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="0" t="n">
         <v>400</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>21</v>
+      <c r="E4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>25</v>
+      <c r="A5" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="0" t="n">
         <v>200</v>
       </c>
-      <c r="D5" s="0" t="s">
-        <v>27</v>
-      </c>
       <c r="E5" s="0" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="H5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="J5" s="0" t="s">
+      <c r="I5" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="K5" s="0" t="n">
+      <c r="J5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="L5" s="0" t="n">
         <v>6543210987</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>33</v>
+      <c r="A6" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="0" t="n">
         <v>200</v>
       </c>
-      <c r="D6" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="G6" s="1" t="s">
+      <c r="E6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="0" t="s">
+      <c r="G6" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="H6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="J6" s="0" t="s">
+      <c r="I6" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="K6" s="0" t="n">
+      <c r="J6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="L6" s="0" t="n">
         <v>5432109876</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" display="johndoe@gmail.com"/>
-    <hyperlink ref="I5" r:id="rId2" display="vankat@yahoo.com"/>
-    <hyperlink ref="I6" r:id="rId3" display="helen@ukmail.com"/>
+    <hyperlink ref="J2" r:id="rId1" display="johndoe@gmail.com"/>
+    <hyperlink ref="J5" r:id="rId2" display="vankat@yahoo.com"/>
+    <hyperlink ref="J6" r:id="rId3" display="helen@ukmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>